<commit_message>
Fixed the Data sheet path
</commit_message>
<xml_diff>
--- a/src/test/java/com/test/LoginData.xlsx
+++ b/src/test/java/com/test/LoginData.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="330" windowWidth="16890" windowHeight="3000"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="16560" windowHeight="6420"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
   <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Email_ID</t>
   </si>
@@ -29,6 +29,12 @@
   </si>
   <si>
     <t>Hello@123</t>
+  </si>
+  <si>
+    <t>syed_hussain@hcl.com</t>
+  </si>
+  <si>
+    <t>hhhjjj</t>
   </si>
 </sst>
 </file>
@@ -388,9 +394,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -414,13 +422,22 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="A3" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>